<commit_message>
doc - improve IMPORT & METAMODEL
</commit_message>
<xml_diff>
--- a/docs/excel-import/samples/Invest_And_Securities_Landscape.xlsx
+++ b/docs/excel-import/samples/Invest_And_Securities_Landscape.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
   <si>
     <t xml:space="preserve">From ADD</t>
   </si>
@@ -237,6 +237,39 @@
   </si>
   <si>
     <t xml:space="preserve">Send accounting information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAD.006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer synchronization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send Customer in NRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAD.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Microservice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send Customer in batch mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File</t>
   </si>
 </sst>
 </file>
@@ -504,9 +537,9 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,27 +678,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26"/>
@@ -936,6 +969,64 @@
       </c>
       <c r="G9" s="0" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>